<commit_message>
Adapted option to quit session, bug fixes
</commit_message>
<xml_diff>
--- a/OpenDashboard_Configurations.xlsx
+++ b/OpenDashboard_Configurations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8610" windowHeight="3860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8610" windowHeight="3855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SpatialData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>DataName_com</t>
   </si>
@@ -61,34 +61,19 @@
     <t>Stadtteile</t>
   </si>
   <si>
-    <t>EW_Altersklassen</t>
-  </si>
-  <si>
-    <t>BundesagenturArbeitNov.2015</t>
-  </si>
-  <si>
-    <t>BundesagenturFuerArbeit</t>
+    <t>JoinField</t>
+  </si>
+  <si>
+    <t>BundesagenturArbeit_link</t>
+  </si>
+  <si>
+    <t>BundesagenturArbeit_link.xlsx</t>
+  </si>
+  <si>
+    <t>BundesagenturArbeit</t>
   </si>
   <si>
     <t>Bundesagentur für Arbeit</t>
-  </si>
-  <si>
-    <t>Familien</t>
-  </si>
-  <si>
-    <t>EW_Altersklassen.xlsx</t>
-  </si>
-  <si>
-    <t>BundesagenturArbeitNov.2015.xlsx</t>
-  </si>
-  <si>
-    <t>Familien.xlsx</t>
-  </si>
-  <si>
-    <t>Altersklassen</t>
-  </si>
-  <si>
-    <t>JoinField</t>
   </si>
 </sst>
 </file>
@@ -432,16 +417,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.90625" style="2"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -483,7 +468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -507,19 +492,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,47 +518,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -584,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Major bug fixes and some new features
</commit_message>
<xml_diff>
--- a/OpenDashboard_Configurations.xlsx
+++ b/OpenDashboard_Configurations.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>DataName_com</t>
   </si>
@@ -74,6 +74,48 @@
   </si>
   <si>
     <t>Bundesagentur für Arbeit</t>
+  </si>
+  <si>
+    <t>EW_Altersklassen_link</t>
+  </si>
+  <si>
+    <t>EW_Altersklassen_link.xlsx</t>
+  </si>
+  <si>
+    <t>EW Altersklassen</t>
+  </si>
+  <si>
+    <t>Familien_link</t>
+  </si>
+  <si>
+    <t>Familien_link.xlsx</t>
+  </si>
+  <si>
+    <t>Familien</t>
+  </si>
+  <si>
+    <t>EW_Altersklassen</t>
+  </si>
+  <si>
+    <t>FlaecheDichte</t>
+  </si>
+  <si>
+    <t>Flächen und Dichten</t>
+  </si>
+  <si>
+    <t>FlaecheDichte_link.xlsx</t>
+  </si>
+  <si>
+    <t>FlaecheDichte_link</t>
+  </si>
+  <si>
+    <t>Wanderungen</t>
+  </si>
+  <si>
+    <t>Wanderungen_link.xlsx</t>
+  </si>
+  <si>
+    <t>Wanderungen_link</t>
   </si>
 </sst>
 </file>
@@ -490,10 +532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,16 +575,60 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>